<commit_message>
New script and code change for ExcelUtilities class
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav\Desktop\SelemiumJavaTestingProject2025\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E463C504-45A1-4456-A8DD-1CEF23049782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BAEE37-1811-4510-AA5D-0A37EFE5A478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>FirstName</t>
   </si>
@@ -53,12 +53,6 @@
     <t>More</t>
   </si>
   <si>
-    <t>vaibhav@example.com</t>
-  </si>
-  <si>
-    <t>9876543210</t>
-  </si>
-  <si>
     <t>Engineer</t>
   </si>
   <si>
@@ -68,13 +62,25 @@
     <t>Pass@123</t>
   </si>
   <si>
-    <t>Tore</t>
-  </si>
-  <si>
-    <t>vaibhav11@example.com</t>
-  </si>
-  <si>
     <t>Pass@1234</t>
+  </si>
+  <si>
+    <t>8876543210</t>
+  </si>
+  <si>
+    <t>Rgghav</t>
+  </si>
+  <si>
+    <t>Raghav11@example.com</t>
+  </si>
+  <si>
+    <t>otte</t>
+  </si>
+  <si>
+    <t>vaibhavotte511@example.com</t>
+  </si>
+  <si>
+    <t>7476543215</t>
   </si>
 </sst>
 </file>
@@ -119,9 +125,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,7 +435,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,31 +468,34 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8C0859B3-358D-4BB2-A85D-01EAE33420F5}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -534,25 +544,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2">
-        <v>9576543210</v>
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new pageObject classes for test script PlaceOrderAndVerifyByOrderIDTest
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav\Desktop\SelemiumJavaTestingProject2025\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BAEE37-1811-4510-AA5D-0A37EFE5A478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C0DE75-40D0-47E9-9C59-56C29FEF8717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
     <sheet name="NewUserRegister" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductOrderList" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -81,13 +83,34 @@
   </si>
   <si>
     <t>7476543215</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ADIDAS ORIGINAL</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>NameOnCard</t>
+  </si>
+  <si>
+    <t>anshika</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +125,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,10 +155,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -504,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC6A7BC-31A1-4867-A5B0-82AA0620E4EB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -573,4 +606,50 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687251BB-4F80-4762-BD6A-9B098E5EF8D9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>911</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>